<commit_message>
Finalizando módulo 11 e iniciando Módulo 12 - Macros
</commit_message>
<xml_diff>
--- a/Modulo 11 - Fórmulas avançadas/aula-desloc-corresp.xlsx
+++ b/Modulo 11 - Fórmulas avançadas/aula-desloc-corresp.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20404"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88D4B07-7309-481A-9BDA-68EB0186F318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estados" sheetId="1" r:id="rId1"/>
@@ -12,18 +13,17 @@
     <sheet name="Repasses" sheetId="3" r:id="rId3"/>
     <sheet name="Testes" sheetId="4" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="TbCidades_Cidade">[1]!TbCidades[Cidade]</definedName>
+    <definedName name="TbCidades_Cidade">TbCidades[Cidade]</definedName>
+    <definedName name="TbCidades_Estado">TbCidades[Estado]</definedName>
+    <definedName name="TbEstados_Estado">TbEstados[Estado]</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
   <si>
     <t>Estado</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Classificação</t>
-  </si>
-  <si>
-    <t>Secundárias</t>
   </si>
   <si>
     <t>DESLOC</t>
@@ -130,9 +127,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -219,7 +216,7 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -253,7 +250,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -268,55 +265,34 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Estados"/>
-      <sheetName val="Cidades"/>
-      <sheetName val="Repasses"/>
-      <sheetName val="Testes"/>
-      <sheetName val="aula-desloc-corresp_GABARITO"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbEstados" displayName="TbEstados" ref="A1:A6" totalsRowShown="0">
-  <autoFilter ref="A1:A6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TbEstados" displayName="TbEstados" ref="A1:A6" totalsRowShown="0">
+  <autoFilter ref="A1:A6" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Estado"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Estado"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TbCidades" displayName="TbCidades" ref="A1:B16" totalsRowShown="0">
-  <autoFilter ref="A1:B16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TbCidades" displayName="TbCidades" ref="A1:B16" totalsRowShown="0">
+  <autoFilter ref="A1:B16" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Estado"/>
-    <tableColumn id="2" name="Cidade"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Estado"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cidade"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbRepasses" displayName="TbRepasses" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TbRepasses" displayName="TbRepasses" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Estado"/>
-    <tableColumn id="2" name="Cidade"/>
-    <tableColumn id="3" name="Valor do repasse" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Estado"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Cidade"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Valor do repasse" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -325,7 +301,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -363,7 +339,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -398,6 +374,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -433,9 +426,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -608,42 +618,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -657,20 +669,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" style="2" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -686,11 +700,11 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -701,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -710,7 +724,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -718,20 +732,23 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <f>MATCH(D3,TbCidades_Estado,0)</f>
+        <v>3</v>
+      </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -739,7 +756,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -747,19 +764,22 @@
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="3">
+        <f>COUNTIF(TbCidades_Estado,D3)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -767,7 +787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -775,7 +795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -783,7 +803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -791,7 +811,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -799,7 +819,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -807,7 +827,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -816,6 +836,17 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{C47E048C-6C09-421A-883E-69AD7E8D7559}">
+      <formula1>OFFSET(TbCidades_Cidade,4,0,2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4" xr:uid="{75560BAE-875A-4675-AAC1-8F7C550037FC}">
+      <formula1>OFFSET(TbCidades_Cidade,D6-1,0,3)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6" xr:uid="{8537A568-F797-4EF0-8B4A-34E7820C6AB3}">
+      <formula1>OFFSET(TbCidades_Cidade,D6-1,0,D9)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -824,19 +855,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -847,7 +880,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -858,7 +891,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -869,7 +902,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -880,7 +913,37 @@
         <v>40000</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1">
+        <v>50000</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A6" xr:uid="{22998D6F-2117-478E-ADA9-EDE1F34C54D9}">
+      <formula1>TbEstados_Estado</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6" xr:uid="{89671026-6DC5-4708-B567-840ABEA6DAAC}">
+      <formula1>OFFSET(TbCidades_Cidade, MATCH(A2,TbCidades_Estado,0)-1,0, COUNTIF(TbCidades_Estado,A2))</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -889,124 +952,130 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="20.26953125" customWidth="1"/>
+    <col min="6" max="6" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="8">
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>30</v>
       </c>
       <c r="B4" s="8">
         <v>3</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="5">
+        <f ca="1">SUM(OFFSET(A5,0,1,3))</f>
+        <v>15</v>
+      </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="8">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="8">
         <v>6</v>
       </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="6">
+        <f>MATCH(F4,A2:A11,)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="9">
         <v>10</v>

</xml_diff>